<commit_message>
feat: add sponsor column support for sessions
- Add 'Sponsor' column mapping to SESSION_FIELD_MAPPING in config.py
- Add parse_and_slugify_sponsors() utility function to convert sponsor names to slugs
- Update data processor to extract and parse sponsor data from Excel
- Update session generator to include sponsors in YAML frontmatter when present
- Add sponsor extraction and comparison logic for content verification
- Sponsors are only included in YAML when they exist (no empty fields)
- Support comma-separated sponsor values with proper slug conversion
- Add sponsor change detection for session updates

Example output:
sponsors:
- 'elasticscale'
- 'palo-alto-networks'
</commit_message>
<xml_diff>
--- a/samples/responses+votes.xlsx
+++ b/samples/responses+votes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ndewijer/Github/ndewijer/Communityday-hugo-speaker-generator/samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ndewijer/Github/ndewijer/communityday-hugo-speaker-generator/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551DEC84-1980-274D-99E6-63240239B58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974902B2-D1B0-A645-B4D8-FB89429F5219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44940" yWindow="-14860" windowWidth="23140" windowHeight="17820" xr2:uid="{82BC87B7-539C-914B-9C85-368574C9C29A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{82BC87B7-539C-914B-9C85-368574C9C29A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="139">
   <si>
     <t>Session_ID</t>
   </si>
@@ -426,13 +426,40 @@
   </si>
   <si>
     <t>Link to photo (Optional, defaults to LinkedIn Profile)</t>
+  </si>
+  <si>
+    <t>VOTES</t>
+  </si>
+  <si>
+    <t>SESSION PLACEMENT</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Agenda</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>elastic</t>
+  </si>
+  <si>
+    <t>starfleet</t>
+  </si>
+  <si>
+    <t>SUBMISSION</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -446,6 +473,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -455,7 +496,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -463,12 +504,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,1365 +937,1632 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58DFE803-2416-344A-BC48-87F14A4A78F2}">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="87.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="50.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="193.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.1640625" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="96.5" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="65.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="87.1640625" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="19" width="19" customWidth="1"/>
+    <col min="20" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.33203125" customWidth="1"/>
+    <col min="26" max="26" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="Z1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>100</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>124</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>99</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>128</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>77</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
       <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2">
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="S2" s="4"/>
+      <c r="T2">
         <v>5</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>12</v>
       </c>
-      <c r="S2">
+      <c r="V2">
         <v>18</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>15</v>
       </c>
-      <c r="U2">
+      <c r="X2" s="5">
         <v>5</v>
       </c>
+      <c r="Z2" s="4"/>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>1300</v>
+      </c>
+      <c r="AC2" s="5"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>124</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>99</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>78</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>76</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="Q3">
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="S3" s="4"/>
+      <c r="T3">
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="U3">
         <v>14</v>
       </c>
-      <c r="S3">
+      <c r="V3">
         <v>18</v>
       </c>
-      <c r="T3">
+      <c r="W3">
         <v>13</v>
       </c>
-      <c r="U3">
+      <c r="X3" s="5">
         <v>3</v>
       </c>
+      <c r="Z3" s="4"/>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1100</v>
+      </c>
+      <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>103</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>100</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>124</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>99</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>79</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>76</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>30</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
       <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="Q4">
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="S4" s="4"/>
+      <c r="T4">
         <v>5</v>
       </c>
-      <c r="R4">
+      <c r="U4">
         <v>12</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>18</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>13</v>
       </c>
-      <c r="U4">
+      <c r="X4" s="5">
         <v>5</v>
       </c>
+      <c r="Z4" s="4"/>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1300</v>
+      </c>
+      <c r="AC4" s="5"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>123</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>104</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>124</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>99</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>80</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>76</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>29</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>23</v>
       </c>
-      <c r="M5" t="s">
-        <v>24</v>
-      </c>
       <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="Q5">
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="S5" s="4"/>
+      <c r="T5">
         <v>5</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>11</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>17</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>13</v>
       </c>
-      <c r="U5">
+      <c r="X5" s="5">
         <v>4</v>
       </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5">
+        <v>5</v>
+      </c>
+      <c r="AB5">
+        <v>1630</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>123</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>105</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>100</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>124</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>99</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>81</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>76</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>29</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>34</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>35</v>
       </c>
-      <c r="M6" t="s">
-        <v>24</v>
-      </c>
       <c r="N6" t="s">
         <v>24</v>
       </c>
-      <c r="Q6">
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="S6" s="4"/>
+      <c r="T6">
         <v>4</v>
       </c>
-      <c r="R6">
+      <c r="U6">
         <v>9</v>
       </c>
-      <c r="S6">
+      <c r="V6">
         <v>19</v>
       </c>
-      <c r="T6">
+      <c r="W6">
         <v>12</v>
       </c>
-      <c r="U6">
+      <c r="X6" s="5">
         <v>5</v>
       </c>
+      <c r="Z6" s="4"/>
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AB6">
+        <v>1100</v>
+      </c>
+      <c r="AC6" s="5"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>123</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>106</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>100</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>124</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>99</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>128</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>82</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>76</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>21</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>37</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>38</v>
       </c>
-      <c r="M7" t="s">
-        <v>24</v>
-      </c>
       <c r="N7" t="s">
         <v>24</v>
       </c>
-      <c r="Q7">
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="S7" s="4"/>
+      <c r="T7">
         <v>5</v>
       </c>
-      <c r="R7">
+      <c r="U7">
         <v>10</v>
       </c>
-      <c r="S7">
+      <c r="V7">
         <v>17</v>
       </c>
-      <c r="T7">
+      <c r="W7">
         <v>12</v>
       </c>
-      <c r="U7">
+      <c r="X7" s="5">
         <v>3</v>
       </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="AC7" s="5"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>123</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>107</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>100</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>124</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>99</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>83</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>76</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>21</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>40</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>38</v>
       </c>
-      <c r="M8" t="s">
-        <v>24</v>
-      </c>
       <c r="N8" t="s">
         <v>24</v>
       </c>
-      <c r="Q8">
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="S8" s="4"/>
+      <c r="T8">
         <v>3</v>
       </c>
-      <c r="R8">
+      <c r="U8">
         <v>15</v>
       </c>
-      <c r="S8">
+      <c r="V8">
         <v>15</v>
       </c>
-      <c r="T8">
+      <c r="W8">
         <v>11</v>
       </c>
-      <c r="U8">
+      <c r="X8" s="5">
         <v>4</v>
       </c>
+      <c r="Z8" s="4"/>
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>1530</v>
+      </c>
+      <c r="AC8" s="5"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>123</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>108</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>100</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>124</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>99</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>84</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>29</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>42</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>23</v>
       </c>
-      <c r="M9" t="s">
-        <v>24</v>
-      </c>
       <c r="N9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
         <v>43</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>125</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q9">
+      <c r="S9" s="4"/>
+      <c r="T9">
         <v>4</v>
       </c>
-      <c r="R9">
+      <c r="U9">
         <v>12</v>
       </c>
-      <c r="S9">
+      <c r="V9">
         <v>12</v>
       </c>
-      <c r="T9">
+      <c r="W9">
         <v>11</v>
       </c>
-      <c r="U9">
+      <c r="X9" s="5">
         <v>1</v>
       </c>
+      <c r="Z9" s="4"/>
+      <c r="AA9">
+        <v>3</v>
+      </c>
+      <c r="AB9">
+        <v>1500</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>123</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>109</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>100</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>124</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>99</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>128</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>85</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>76</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>21</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>46</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>38</v>
       </c>
-      <c r="M10" t="s">
-        <v>24</v>
-      </c>
       <c r="N10" t="s">
         <v>24</v>
       </c>
-      <c r="Q10">
+      <c r="O10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="S10" s="4"/>
+      <c r="T10">
         <v>4</v>
       </c>
-      <c r="R10">
+      <c r="U10">
         <v>7</v>
       </c>
-      <c r="S10">
+      <c r="V10">
         <v>18</v>
       </c>
-      <c r="T10">
+      <c r="W10">
         <v>13</v>
       </c>
-      <c r="U10">
+      <c r="X10" s="5">
         <v>4</v>
       </c>
+      <c r="Z10" s="4"/>
+      <c r="AA10">
+        <v>2</v>
+      </c>
+      <c r="AB10">
+        <v>1100</v>
+      </c>
+      <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>123</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>110</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>100</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>124</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>99</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>86</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>76</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>21</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>48</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>23</v>
       </c>
-      <c r="M11" t="s">
-        <v>24</v>
-      </c>
       <c r="N11" t="s">
         <v>24</v>
       </c>
-      <c r="Q11">
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="S11" s="4"/>
+      <c r="T11">
         <v>4</v>
       </c>
-      <c r="R11">
+      <c r="U11">
         <v>14</v>
       </c>
-      <c r="S11">
+      <c r="V11">
         <v>15</v>
       </c>
-      <c r="T11">
+      <c r="W11">
         <v>10</v>
       </c>
-      <c r="U11">
+      <c r="X11" s="5">
         <v>5</v>
       </c>
+      <c r="Z11" s="4"/>
+      <c r="AA11">
+        <v>4</v>
+      </c>
+      <c r="AB11">
+        <v>1100</v>
+      </c>
+      <c r="AC11" s="5"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>123</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>100</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>124</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>99</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>87</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>76</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>21</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>50</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>38</v>
       </c>
-      <c r="M12" t="s">
-        <v>24</v>
-      </c>
       <c r="N12" t="s">
         <v>24</v>
       </c>
-      <c r="Q12">
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="S12" s="4"/>
+      <c r="T12">
         <v>5</v>
       </c>
-      <c r="R12">
+      <c r="U12">
         <v>9</v>
       </c>
-      <c r="S12">
+      <c r="V12">
         <v>17</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>13</v>
       </c>
-      <c r="U12">
+      <c r="X12" s="5">
         <v>3</v>
       </c>
+      <c r="Z12" s="4"/>
+      <c r="AA12">
+        <v>4</v>
+      </c>
+      <c r="AB12">
+        <v>1300</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>123</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>100</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>124</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>99</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>88</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>76</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>52</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>23</v>
       </c>
-      <c r="M13" t="s">
-        <v>24</v>
-      </c>
       <c r="N13" t="s">
         <v>24</v>
       </c>
-      <c r="P13" t="s">
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q13">
+      <c r="S13" s="4"/>
+      <c r="T13">
         <v>5</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>10</v>
       </c>
-      <c r="S13">
+      <c r="V13">
         <v>16</v>
       </c>
-      <c r="T13">
+      <c r="W13">
         <v>14</v>
       </c>
-      <c r="U13">
+      <c r="X13" s="5">
         <v>4</v>
       </c>
+      <c r="Z13" s="4"/>
+      <c r="AA13">
+        <v>5</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>1300</v>
+      </c>
+      <c r="AC13" s="5"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>123</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>100</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>124</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>99</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>89</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>76</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>26</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>55</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>23</v>
       </c>
-      <c r="M14" t="s">
-        <v>24</v>
-      </c>
       <c r="N14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" t="s">
         <v>43</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>126</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="5"/>
+      <c r="S14" s="4"/>
+      <c r="T14">
         <v>4</v>
       </c>
-      <c r="R14">
+      <c r="U14">
         <v>14</v>
       </c>
-      <c r="S14">
+      <c r="V14">
         <v>19</v>
       </c>
-      <c r="T14">
+      <c r="W14">
         <v>14</v>
       </c>
-      <c r="U14">
+      <c r="X14" s="5">
         <v>4</v>
       </c>
+      <c r="Z14" s="4"/>
+      <c r="AA14">
+        <v>3</v>
+      </c>
+      <c r="AB14">
+        <v>1630</v>
+      </c>
+      <c r="AC14" s="5"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>123</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>114</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>100</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>124</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>99</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>90</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>76</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>57</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>58</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>23</v>
       </c>
-      <c r="M15" t="s">
-        <v>24</v>
-      </c>
       <c r="N15" t="s">
         <v>24</v>
       </c>
-      <c r="P15" t="s">
+      <c r="O15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q15">
+      <c r="S15" s="4"/>
+      <c r="T15">
         <v>4</v>
       </c>
-      <c r="R15">
+      <c r="U15">
         <v>18</v>
       </c>
-      <c r="S15">
+      <c r="V15">
         <v>20</v>
       </c>
-      <c r="T15">
+      <c r="W15">
         <v>11</v>
       </c>
-      <c r="U15">
+      <c r="X15" s="5">
         <v>5</v>
       </c>
+      <c r="Z15" s="4"/>
+      <c r="AA15">
+        <v>5</v>
+      </c>
+      <c r="AB15">
+        <v>1130</v>
+      </c>
+      <c r="AC15" s="5"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>123</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>115</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>100</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>124</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>99</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>91</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>76</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>57</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>60</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>38</v>
       </c>
-      <c r="M16" t="s">
-        <v>24</v>
-      </c>
       <c r="N16" t="s">
         <v>24</v>
       </c>
-      <c r="P16" t="s">
+      <c r="O16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q16">
+      <c r="S16" s="4"/>
+      <c r="T16">
         <v>4</v>
       </c>
-      <c r="R16">
+      <c r="U16">
         <v>17</v>
       </c>
-      <c r="S16">
+      <c r="V16">
         <v>20</v>
       </c>
-      <c r="T16">
+      <c r="W16">
         <v>14</v>
       </c>
-      <c r="U16">
+      <c r="X16" s="5">
         <v>2</v>
       </c>
+      <c r="Z16" s="4"/>
+      <c r="AA16">
+        <v>2</v>
+      </c>
+      <c r="AB16">
+        <v>1500</v>
+      </c>
+      <c r="AC16" s="5"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>123</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>116</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>100</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>124</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>99</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>92</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>76</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>21</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>62</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>38</v>
       </c>
-      <c r="M17" t="s">
-        <v>24</v>
-      </c>
       <c r="N17" t="s">
         <v>24</v>
       </c>
-      <c r="P17" t="s">
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q17">
+      <c r="S17" s="4"/>
+      <c r="T17">
         <v>4</v>
       </c>
-      <c r="R17">
+      <c r="U17">
         <v>8</v>
       </c>
-      <c r="S17">
+      <c r="V17">
         <v>20</v>
       </c>
-      <c r="T17">
+      <c r="W17">
         <v>12</v>
       </c>
-      <c r="U17">
+      <c r="X17" s="5">
         <v>2</v>
       </c>
+      <c r="Z17" s="4"/>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>1500</v>
+      </c>
+      <c r="AC17" s="5"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" t="s">
         <v>63</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>123</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>117</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>100</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>124</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>99</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>93</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>76</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>29</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>64</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>38</v>
       </c>
-      <c r="M18" t="s">
-        <v>24</v>
-      </c>
       <c r="N18" t="s">
         <v>24</v>
       </c>
-      <c r="P18" t="s">
+      <c r="O18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q18">
+      <c r="S18" s="4"/>
+      <c r="T18">
         <v>4</v>
       </c>
-      <c r="R18">
+      <c r="U18">
         <v>12</v>
       </c>
-      <c r="S18">
+      <c r="V18">
         <v>20</v>
       </c>
-      <c r="T18">
+      <c r="W18">
         <v>12</v>
       </c>
-      <c r="U18">
+      <c r="X18" s="5">
         <v>3</v>
       </c>
+      <c r="Z18" s="4"/>
+      <c r="AA18">
+        <v>5</v>
+      </c>
+      <c r="AB18">
+        <v>1100</v>
+      </c>
+      <c r="AC18" s="5"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>123</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>118</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>100</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>124</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>99</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>94</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>76</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>29</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>67</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>38</v>
       </c>
-      <c r="M19" t="s">
-        <v>24</v>
-      </c>
       <c r="N19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" t="s">
         <v>43</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>127</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="5"/>
+      <c r="S19" s="4"/>
+      <c r="T19">
         <v>5</v>
       </c>
-      <c r="R19">
+      <c r="U19">
         <v>9</v>
       </c>
-      <c r="S19">
+      <c r="V19">
         <v>16</v>
       </c>
-      <c r="T19">
+      <c r="W19">
         <v>12</v>
       </c>
-      <c r="U19">
+      <c r="X19" s="5">
         <v>3</v>
       </c>
+      <c r="Z19" s="4"/>
+      <c r="AA19">
+        <v>4</v>
+      </c>
+      <c r="AB19">
+        <v>1500</v>
+      </c>
+      <c r="AC19" s="5"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>123</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>119</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>100</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>124</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>99</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>95</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>76</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>29</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>69</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>38</v>
       </c>
-      <c r="M20" t="s">
-        <v>24</v>
-      </c>
       <c r="N20" t="s">
         <v>24</v>
       </c>
-      <c r="Q20">
+      <c r="O20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q20" s="5"/>
+      <c r="S20" s="4"/>
+      <c r="T20">
         <v>5</v>
       </c>
-      <c r="R20">
+      <c r="U20">
         <v>13</v>
       </c>
-      <c r="S20">
+      <c r="V20">
         <v>18</v>
       </c>
-      <c r="T20">
+      <c r="W20">
         <v>11</v>
       </c>
-      <c r="U20">
+      <c r="X20" s="5">
         <v>4</v>
       </c>
+      <c r="Z20" s="4"/>
+      <c r="AA20">
+        <v>5</v>
+      </c>
+      <c r="AB20">
+        <v>1600</v>
+      </c>
+      <c r="AC20" s="5"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>123</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>120</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>100</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>124</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>99</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>96</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>76</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>26</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>71</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>35</v>
-      </c>
-      <c r="M21" t="s">
-        <v>43</v>
       </c>
       <c r="N21" t="s">
         <v>43</v>
       </c>
-      <c r="Q21">
+      <c r="O21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q21" s="5"/>
+      <c r="S21" s="4"/>
+      <c r="T21">
         <v>5</v>
       </c>
-      <c r="R21">
+      <c r="U21">
         <v>15</v>
       </c>
-      <c r="S21">
+      <c r="V21">
         <v>20</v>
       </c>
-      <c r="T21">
+      <c r="W21">
         <v>14</v>
       </c>
-      <c r="U21">
+      <c r="X21" s="5">
         <v>2</v>
       </c>
+      <c r="Z21" s="4"/>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>1600</v>
+      </c>
+      <c r="AC21" s="5"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>123</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>121</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>100</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>124</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>99</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>97</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>76</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>26</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>73</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>23</v>
-      </c>
-      <c r="M22" t="s">
-        <v>43</v>
       </c>
       <c r="N22" t="s">
         <v>43</v>
       </c>
-      <c r="Q22">
+      <c r="O22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q22" s="5"/>
+      <c r="S22" s="4"/>
+      <c r="T22">
         <v>4</v>
       </c>
-      <c r="R22">
+      <c r="U22">
         <v>17</v>
       </c>
-      <c r="S22">
+      <c r="V22">
         <v>20</v>
       </c>
-      <c r="T22">
+      <c r="W22">
         <v>13</v>
       </c>
-      <c r="U22">
+      <c r="X22" s="5">
         <v>4</v>
       </c>
+      <c r="Z22" s="4"/>
+      <c r="AA22">
+        <v>3</v>
+      </c>
+      <c r="AB22">
+        <v>1300</v>
+      </c>
+      <c r="AC22" s="5"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Q23">
+      <c r="P23" s="7"/>
+      <c r="Q23" s="8"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="7">
         <v>3</v>
       </c>
-      <c r="R23">
+      <c r="U23" s="7">
         <v>14</v>
       </c>
-      <c r="S23">
+      <c r="V23" s="7">
         <v>17</v>
       </c>
-      <c r="T23">
+      <c r="W23" s="7">
         <v>14</v>
       </c>
-      <c r="U23">
+      <c r="X23" s="8">
         <v>4</v>
       </c>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>1400</v>
+      </c>
+      <c r="AC23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat: add sponsor column support for sessions (#11)
- Add 'Sponsor' column mapping to SESSION_FIELD_MAPPING in config.py
- Add parse_and_slugify_sponsors() utility function to convert sponsor names to slugs
- Update data processor to extract and parse sponsor data from Excel
- Update session generator to include sponsors in YAML frontmatter when present
- Add sponsor extraction and comparison logic for content verification
- Sponsors are only included in YAML when they exist (no empty fields)
- Support comma-separated sponsor values with proper slug conversion
- Add sponsor change detection for session updates

Example output:
sponsors:
- 'elasticscale'
- 'palo-alto-networks'
</commit_message>
<xml_diff>
--- a/samples/responses+votes.xlsx
+++ b/samples/responses+votes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ndewijer/Github/ndewijer/Communityday-hugo-speaker-generator/samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ndewijer/Github/ndewijer/communityday-hugo-speaker-generator/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551DEC84-1980-274D-99E6-63240239B58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974902B2-D1B0-A645-B4D8-FB89429F5219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44940" yWindow="-14860" windowWidth="23140" windowHeight="17820" xr2:uid="{82BC87B7-539C-914B-9C85-368574C9C29A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{82BC87B7-539C-914B-9C85-368574C9C29A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="139">
   <si>
     <t>Session_ID</t>
   </si>
@@ -426,13 +426,40 @@
   </si>
   <si>
     <t>Link to photo (Optional, defaults to LinkedIn Profile)</t>
+  </si>
+  <si>
+    <t>VOTES</t>
+  </si>
+  <si>
+    <t>SESSION PLACEMENT</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Agenda</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>elastic</t>
+  </si>
+  <si>
+    <t>starfleet</t>
+  </si>
+  <si>
+    <t>SUBMISSION</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -446,6 +473,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -455,7 +496,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -463,12 +504,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,1365 +937,1632 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58DFE803-2416-344A-BC48-87F14A4A78F2}">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="87.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="50.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="193.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.1640625" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="96.5" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="65.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="87.1640625" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="19" width="19" customWidth="1"/>
+    <col min="20" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.33203125" customWidth="1"/>
+    <col min="26" max="26" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="Z1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>100</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>124</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>99</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>128</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>77</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
       <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2">
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="S2" s="4"/>
+      <c r="T2">
         <v>5</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>12</v>
       </c>
-      <c r="S2">
+      <c r="V2">
         <v>18</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>15</v>
       </c>
-      <c r="U2">
+      <c r="X2" s="5">
         <v>5</v>
       </c>
+      <c r="Z2" s="4"/>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>1300</v>
+      </c>
+      <c r="AC2" s="5"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>124</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>99</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>78</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>76</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="Q3">
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="S3" s="4"/>
+      <c r="T3">
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="U3">
         <v>14</v>
       </c>
-      <c r="S3">
+      <c r="V3">
         <v>18</v>
       </c>
-      <c r="T3">
+      <c r="W3">
         <v>13</v>
       </c>
-      <c r="U3">
+      <c r="X3" s="5">
         <v>3</v>
       </c>
+      <c r="Z3" s="4"/>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1100</v>
+      </c>
+      <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>103</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>100</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>124</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>99</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>79</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>76</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>30</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
       <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="Q4">
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="S4" s="4"/>
+      <c r="T4">
         <v>5</v>
       </c>
-      <c r="R4">
+      <c r="U4">
         <v>12</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>18</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>13</v>
       </c>
-      <c r="U4">
+      <c r="X4" s="5">
         <v>5</v>
       </c>
+      <c r="Z4" s="4"/>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1300</v>
+      </c>
+      <c r="AC4" s="5"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>123</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>104</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>124</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>99</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>80</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>76</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>29</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>23</v>
       </c>
-      <c r="M5" t="s">
-        <v>24</v>
-      </c>
       <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="Q5">
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="S5" s="4"/>
+      <c r="T5">
         <v>5</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>11</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>17</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>13</v>
       </c>
-      <c r="U5">
+      <c r="X5" s="5">
         <v>4</v>
       </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5">
+        <v>5</v>
+      </c>
+      <c r="AB5">
+        <v>1630</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>123</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>105</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>100</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>124</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>99</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>81</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>76</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>29</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>34</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>35</v>
       </c>
-      <c r="M6" t="s">
-        <v>24</v>
-      </c>
       <c r="N6" t="s">
         <v>24</v>
       </c>
-      <c r="Q6">
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="S6" s="4"/>
+      <c r="T6">
         <v>4</v>
       </c>
-      <c r="R6">
+      <c r="U6">
         <v>9</v>
       </c>
-      <c r="S6">
+      <c r="V6">
         <v>19</v>
       </c>
-      <c r="T6">
+      <c r="W6">
         <v>12</v>
       </c>
-      <c r="U6">
+      <c r="X6" s="5">
         <v>5</v>
       </c>
+      <c r="Z6" s="4"/>
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AB6">
+        <v>1100</v>
+      </c>
+      <c r="AC6" s="5"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>123</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>106</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>100</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>124</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>99</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>128</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>82</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>76</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>21</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>37</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>38</v>
       </c>
-      <c r="M7" t="s">
-        <v>24</v>
-      </c>
       <c r="N7" t="s">
         <v>24</v>
       </c>
-      <c r="Q7">
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="S7" s="4"/>
+      <c r="T7">
         <v>5</v>
       </c>
-      <c r="R7">
+      <c r="U7">
         <v>10</v>
       </c>
-      <c r="S7">
+      <c r="V7">
         <v>17</v>
       </c>
-      <c r="T7">
+      <c r="W7">
         <v>12</v>
       </c>
-      <c r="U7">
+      <c r="X7" s="5">
         <v>3</v>
       </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="AC7" s="5"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>123</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>107</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>100</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>124</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>99</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>83</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>76</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>21</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>40</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>38</v>
       </c>
-      <c r="M8" t="s">
-        <v>24</v>
-      </c>
       <c r="N8" t="s">
         <v>24</v>
       </c>
-      <c r="Q8">
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="S8" s="4"/>
+      <c r="T8">
         <v>3</v>
       </c>
-      <c r="R8">
+      <c r="U8">
         <v>15</v>
       </c>
-      <c r="S8">
+      <c r="V8">
         <v>15</v>
       </c>
-      <c r="T8">
+      <c r="W8">
         <v>11</v>
       </c>
-      <c r="U8">
+      <c r="X8" s="5">
         <v>4</v>
       </c>
+      <c r="Z8" s="4"/>
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>1530</v>
+      </c>
+      <c r="AC8" s="5"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>123</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>108</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>100</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>124</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>99</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>84</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>29</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>42</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>23</v>
       </c>
-      <c r="M9" t="s">
-        <v>24</v>
-      </c>
       <c r="N9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
         <v>43</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>125</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q9">
+      <c r="S9" s="4"/>
+      <c r="T9">
         <v>4</v>
       </c>
-      <c r="R9">
+      <c r="U9">
         <v>12</v>
       </c>
-      <c r="S9">
+      <c r="V9">
         <v>12</v>
       </c>
-      <c r="T9">
+      <c r="W9">
         <v>11</v>
       </c>
-      <c r="U9">
+      <c r="X9" s="5">
         <v>1</v>
       </c>
+      <c r="Z9" s="4"/>
+      <c r="AA9">
+        <v>3</v>
+      </c>
+      <c r="AB9">
+        <v>1500</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>123</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>109</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>100</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>124</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>99</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>128</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>85</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>76</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>21</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>46</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>38</v>
       </c>
-      <c r="M10" t="s">
-        <v>24</v>
-      </c>
       <c r="N10" t="s">
         <v>24</v>
       </c>
-      <c r="Q10">
+      <c r="O10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="S10" s="4"/>
+      <c r="T10">
         <v>4</v>
       </c>
-      <c r="R10">
+      <c r="U10">
         <v>7</v>
       </c>
-      <c r="S10">
+      <c r="V10">
         <v>18</v>
       </c>
-      <c r="T10">
+      <c r="W10">
         <v>13</v>
       </c>
-      <c r="U10">
+      <c r="X10" s="5">
         <v>4</v>
       </c>
+      <c r="Z10" s="4"/>
+      <c r="AA10">
+        <v>2</v>
+      </c>
+      <c r="AB10">
+        <v>1100</v>
+      </c>
+      <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>123</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>110</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>100</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>124</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>99</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>86</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>76</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>21</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>48</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>23</v>
       </c>
-      <c r="M11" t="s">
-        <v>24</v>
-      </c>
       <c r="N11" t="s">
         <v>24</v>
       </c>
-      <c r="Q11">
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="S11" s="4"/>
+      <c r="T11">
         <v>4</v>
       </c>
-      <c r="R11">
+      <c r="U11">
         <v>14</v>
       </c>
-      <c r="S11">
+      <c r="V11">
         <v>15</v>
       </c>
-      <c r="T11">
+      <c r="W11">
         <v>10</v>
       </c>
-      <c r="U11">
+      <c r="X11" s="5">
         <v>5</v>
       </c>
+      <c r="Z11" s="4"/>
+      <c r="AA11">
+        <v>4</v>
+      </c>
+      <c r="AB11">
+        <v>1100</v>
+      </c>
+      <c r="AC11" s="5"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>123</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>100</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>124</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>99</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>87</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>76</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>21</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>50</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>38</v>
       </c>
-      <c r="M12" t="s">
-        <v>24</v>
-      </c>
       <c r="N12" t="s">
         <v>24</v>
       </c>
-      <c r="Q12">
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="S12" s="4"/>
+      <c r="T12">
         <v>5</v>
       </c>
-      <c r="R12">
+      <c r="U12">
         <v>9</v>
       </c>
-      <c r="S12">
+      <c r="V12">
         <v>17</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>13</v>
       </c>
-      <c r="U12">
+      <c r="X12" s="5">
         <v>3</v>
       </c>
+      <c r="Z12" s="4"/>
+      <c r="AA12">
+        <v>4</v>
+      </c>
+      <c r="AB12">
+        <v>1300</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>123</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>100</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>124</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>99</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>88</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>76</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>52</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>23</v>
       </c>
-      <c r="M13" t="s">
-        <v>24</v>
-      </c>
       <c r="N13" t="s">
         <v>24</v>
       </c>
-      <c r="P13" t="s">
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q13">
+      <c r="S13" s="4"/>
+      <c r="T13">
         <v>5</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>10</v>
       </c>
-      <c r="S13">
+      <c r="V13">
         <v>16</v>
       </c>
-      <c r="T13">
+      <c r="W13">
         <v>14</v>
       </c>
-      <c r="U13">
+      <c r="X13" s="5">
         <v>4</v>
       </c>
+      <c r="Z13" s="4"/>
+      <c r="AA13">
+        <v>5</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>1300</v>
+      </c>
+      <c r="AC13" s="5"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>123</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>100</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>124</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>99</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>89</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>76</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>26</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>55</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>23</v>
       </c>
-      <c r="M14" t="s">
-        <v>24</v>
-      </c>
       <c r="N14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" t="s">
         <v>43</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>126</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="5"/>
+      <c r="S14" s="4"/>
+      <c r="T14">
         <v>4</v>
       </c>
-      <c r="R14">
+      <c r="U14">
         <v>14</v>
       </c>
-      <c r="S14">
+      <c r="V14">
         <v>19</v>
       </c>
-      <c r="T14">
+      <c r="W14">
         <v>14</v>
       </c>
-      <c r="U14">
+      <c r="X14" s="5">
         <v>4</v>
       </c>
+      <c r="Z14" s="4"/>
+      <c r="AA14">
+        <v>3</v>
+      </c>
+      <c r="AB14">
+        <v>1630</v>
+      </c>
+      <c r="AC14" s="5"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>123</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>114</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>100</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>124</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>99</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>90</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>76</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>57</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>58</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>23</v>
       </c>
-      <c r="M15" t="s">
-        <v>24</v>
-      </c>
       <c r="N15" t="s">
         <v>24</v>
       </c>
-      <c r="P15" t="s">
+      <c r="O15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q15">
+      <c r="S15" s="4"/>
+      <c r="T15">
         <v>4</v>
       </c>
-      <c r="R15">
+      <c r="U15">
         <v>18</v>
       </c>
-      <c r="S15">
+      <c r="V15">
         <v>20</v>
       </c>
-      <c r="T15">
+      <c r="W15">
         <v>11</v>
       </c>
-      <c r="U15">
+      <c r="X15" s="5">
         <v>5</v>
       </c>
+      <c r="Z15" s="4"/>
+      <c r="AA15">
+        <v>5</v>
+      </c>
+      <c r="AB15">
+        <v>1130</v>
+      </c>
+      <c r="AC15" s="5"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>123</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>115</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>100</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>124</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>99</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>91</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>76</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>57</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>60</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>38</v>
       </c>
-      <c r="M16" t="s">
-        <v>24</v>
-      </c>
       <c r="N16" t="s">
         <v>24</v>
       </c>
-      <c r="P16" t="s">
+      <c r="O16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q16">
+      <c r="S16" s="4"/>
+      <c r="T16">
         <v>4</v>
       </c>
-      <c r="R16">
+      <c r="U16">
         <v>17</v>
       </c>
-      <c r="S16">
+      <c r="V16">
         <v>20</v>
       </c>
-      <c r="T16">
+      <c r="W16">
         <v>14</v>
       </c>
-      <c r="U16">
+      <c r="X16" s="5">
         <v>2</v>
       </c>
+      <c r="Z16" s="4"/>
+      <c r="AA16">
+        <v>2</v>
+      </c>
+      <c r="AB16">
+        <v>1500</v>
+      </c>
+      <c r="AC16" s="5"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>123</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>116</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>100</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>124</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>99</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>92</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>76</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>21</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>62</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>38</v>
       </c>
-      <c r="M17" t="s">
-        <v>24</v>
-      </c>
       <c r="N17" t="s">
         <v>24</v>
       </c>
-      <c r="P17" t="s">
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q17">
+      <c r="S17" s="4"/>
+      <c r="T17">
         <v>4</v>
       </c>
-      <c r="R17">
+      <c r="U17">
         <v>8</v>
       </c>
-      <c r="S17">
+      <c r="V17">
         <v>20</v>
       </c>
-      <c r="T17">
+      <c r="W17">
         <v>12</v>
       </c>
-      <c r="U17">
+      <c r="X17" s="5">
         <v>2</v>
       </c>
+      <c r="Z17" s="4"/>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>1500</v>
+      </c>
+      <c r="AC17" s="5"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" t="s">
         <v>63</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>123</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>117</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>100</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>124</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>99</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>93</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>76</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>29</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>64</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>38</v>
       </c>
-      <c r="M18" t="s">
-        <v>24</v>
-      </c>
       <c r="N18" t="s">
         <v>24</v>
       </c>
-      <c r="P18" t="s">
+      <c r="O18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q18">
+      <c r="S18" s="4"/>
+      <c r="T18">
         <v>4</v>
       </c>
-      <c r="R18">
+      <c r="U18">
         <v>12</v>
       </c>
-      <c r="S18">
+      <c r="V18">
         <v>20</v>
       </c>
-      <c r="T18">
+      <c r="W18">
         <v>12</v>
       </c>
-      <c r="U18">
+      <c r="X18" s="5">
         <v>3</v>
       </c>
+      <c r="Z18" s="4"/>
+      <c r="AA18">
+        <v>5</v>
+      </c>
+      <c r="AB18">
+        <v>1100</v>
+      </c>
+      <c r="AC18" s="5"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>123</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>118</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>100</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>124</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>99</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>94</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>76</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>29</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>67</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>38</v>
       </c>
-      <c r="M19" t="s">
-        <v>24</v>
-      </c>
       <c r="N19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" t="s">
         <v>43</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>127</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="5"/>
+      <c r="S19" s="4"/>
+      <c r="T19">
         <v>5</v>
       </c>
-      <c r="R19">
+      <c r="U19">
         <v>9</v>
       </c>
-      <c r="S19">
+      <c r="V19">
         <v>16</v>
       </c>
-      <c r="T19">
+      <c r="W19">
         <v>12</v>
       </c>
-      <c r="U19">
+      <c r="X19" s="5">
         <v>3</v>
       </c>
+      <c r="Z19" s="4"/>
+      <c r="AA19">
+        <v>4</v>
+      </c>
+      <c r="AB19">
+        <v>1500</v>
+      </c>
+      <c r="AC19" s="5"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>123</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>119</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>100</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>124</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>99</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>95</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>76</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>29</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>69</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>38</v>
       </c>
-      <c r="M20" t="s">
-        <v>24</v>
-      </c>
       <c r="N20" t="s">
         <v>24</v>
       </c>
-      <c r="Q20">
+      <c r="O20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q20" s="5"/>
+      <c r="S20" s="4"/>
+      <c r="T20">
         <v>5</v>
       </c>
-      <c r="R20">
+      <c r="U20">
         <v>13</v>
       </c>
-      <c r="S20">
+      <c r="V20">
         <v>18</v>
       </c>
-      <c r="T20">
+      <c r="W20">
         <v>11</v>
       </c>
-      <c r="U20">
+      <c r="X20" s="5">
         <v>4</v>
       </c>
+      <c r="Z20" s="4"/>
+      <c r="AA20">
+        <v>5</v>
+      </c>
+      <c r="AB20">
+        <v>1600</v>
+      </c>
+      <c r="AC20" s="5"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>123</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>120</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>100</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>124</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>99</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>96</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>76</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>26</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>71</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>35</v>
-      </c>
-      <c r="M21" t="s">
-        <v>43</v>
       </c>
       <c r="N21" t="s">
         <v>43</v>
       </c>
-      <c r="Q21">
+      <c r="O21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q21" s="5"/>
+      <c r="S21" s="4"/>
+      <c r="T21">
         <v>5</v>
       </c>
-      <c r="R21">
+      <c r="U21">
         <v>15</v>
       </c>
-      <c r="S21">
+      <c r="V21">
         <v>20</v>
       </c>
-      <c r="T21">
+      <c r="W21">
         <v>14</v>
       </c>
-      <c r="U21">
+      <c r="X21" s="5">
         <v>2</v>
       </c>
+      <c r="Z21" s="4"/>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>1600</v>
+      </c>
+      <c r="AC21" s="5"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>123</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>121</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>100</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>124</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>99</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>97</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>76</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>26</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>73</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>23</v>
-      </c>
-      <c r="M22" t="s">
-        <v>43</v>
       </c>
       <c r="N22" t="s">
         <v>43</v>
       </c>
-      <c r="Q22">
+      <c r="O22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q22" s="5"/>
+      <c r="S22" s="4"/>
+      <c r="T22">
         <v>4</v>
       </c>
-      <c r="R22">
+      <c r="U22">
         <v>17</v>
       </c>
-      <c r="S22">
+      <c r="V22">
         <v>20</v>
       </c>
-      <c r="T22">
+      <c r="W22">
         <v>13</v>
       </c>
-      <c r="U22">
+      <c r="X22" s="5">
         <v>4</v>
       </c>
+      <c r="Z22" s="4"/>
+      <c r="AA22">
+        <v>3</v>
+      </c>
+      <c r="AB22">
+        <v>1300</v>
+      </c>
+      <c r="AC22" s="5"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Q23">
+      <c r="P23" s="7"/>
+      <c r="Q23" s="8"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="7">
         <v>3</v>
       </c>
-      <c r="R23">
+      <c r="U23" s="7">
         <v>14</v>
       </c>
-      <c r="S23">
+      <c r="V23" s="7">
         <v>17</v>
       </c>
-      <c r="T23">
+      <c r="W23" s="7">
         <v>14</v>
       </c>
-      <c r="U23">
+      <c r="X23" s="8">
         <v>4</v>
       </c>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>1400</v>
+      </c>
+      <c r="AC23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
docs: update documentation for sponsor column feature
- Add clear distinction between mandatory and optional Excel columns
- Document new Sponsor column functionality with examples
- Add sponsor processing details to Features in Detail section
- Update implementation plan with sponsor field mapping and template
- Clarify sponsor slug conversion and comma-separated value handling
- Maintain concise documentation without verbose YAML examples
</commit_message>
<xml_diff>
--- a/samples/responses+votes.xlsx
+++ b/samples/responses+votes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ndewijer/Github/ndewijer/communityday-hugo-speaker-generator/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974902B2-D1B0-A645-B4D8-FB89429F5219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEA011F-6C69-0049-94D3-B590B206F8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{82BC87B7-539C-914B-9C85-368574C9C29A}"/>
   </bookViews>
@@ -440,12 +440,6 @@
     <t>Agenda</t>
   </si>
   <si>
-    <t>google</t>
-  </si>
-  <si>
-    <t>elastic</t>
-  </si>
-  <si>
     <t>starfleet</t>
   </si>
   <si>
@@ -453,6 +447,12 @@
   </si>
   <si>
     <t>Sponsor</t>
+  </si>
+  <si>
+    <t>google,microsoft</t>
+  </si>
+  <si>
+    <t>elastic, paulo alto</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,7 @@
   <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,11 +967,12 @@
     <col min="20" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.33203125" customWidth="1"/>
     <col min="26" max="26" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1049,7 +1050,7 @@
         <v>133</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -1322,7 +1323,7 @@
         <v>1630</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -1600,7 +1601,7 @@
         <v>1500</v>
       </c>
       <c r="AC9" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -1806,7 +1807,7 @@
         <v>1300</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
docs: update documentation for sponsor column feature (#12)
- Add clear distinction between mandatory and optional Excel columns
- Document new Sponsor column functionality with examples
- Add sponsor processing details to Features in Detail section
- Update implementation plan with sponsor field mapping and template
- Clarify sponsor slug conversion and comma-separated value handling
- Maintain concise documentation without verbose YAML examples
</commit_message>
<xml_diff>
--- a/samples/responses+votes.xlsx
+++ b/samples/responses+votes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ndewijer/Github/ndewijer/communityday-hugo-speaker-generator/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974902B2-D1B0-A645-B4D8-FB89429F5219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEA011F-6C69-0049-94D3-B590B206F8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{82BC87B7-539C-914B-9C85-368574C9C29A}"/>
   </bookViews>
@@ -440,12 +440,6 @@
     <t>Agenda</t>
   </si>
   <si>
-    <t>google</t>
-  </si>
-  <si>
-    <t>elastic</t>
-  </si>
-  <si>
     <t>starfleet</t>
   </si>
   <si>
@@ -453,6 +447,12 @@
   </si>
   <si>
     <t>Sponsor</t>
+  </si>
+  <si>
+    <t>google,microsoft</t>
+  </si>
+  <si>
+    <t>elastic, paulo alto</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,7 @@
   <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,11 +967,12 @@
     <col min="20" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.33203125" customWidth="1"/>
     <col min="26" max="26" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1049,7 +1050,7 @@
         <v>133</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -1322,7 +1323,7 @@
         <v>1630</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -1600,7 +1601,7 @@
         <v>1500</v>
       </c>
       <c r="AC9" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -1806,7 +1807,7 @@
         <v>1300</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>